<commit_message>
converted font 1206 to font 1006 by cutting top 2 bits
</commit_message>
<xml_diff>
--- a/tmp_draw_char.xlsx
+++ b/tmp_draw_char.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E4E5E4-6B5E-4348-99C6-25B9D729A186}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F215C232-24FD-4772-B6DB-03B736676CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="1305" windowWidth="21600" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,447 +407,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1707,7 +1267,7 @@
   <dimension ref="A1:AM30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+      <selection activeCell="AC22" sqref="AC21:AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,234 +2224,234 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:M11 B4:F7 H4:M7">
-    <cfRule type="cellIs" dxfId="101" priority="97" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="97" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="98" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="cellIs" dxfId="99" priority="95" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="95" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="96" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:B22">
-    <cfRule type="cellIs" dxfId="97" priority="93" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="93" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="94" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="95" priority="91" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="91" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="92" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="93" priority="89" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="89" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="90" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B30">
-    <cfRule type="cellIs" dxfId="91" priority="87" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="87" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="88" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:T30">
-    <cfRule type="cellIs" dxfId="89" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB15:AG18">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C19">
-    <cfRule type="cellIs" dxfId="83" priority="83" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="83" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="84" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C22">
-    <cfRule type="cellIs" dxfId="81" priority="81" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="81" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C24">
-    <cfRule type="cellIs" dxfId="79" priority="79" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="80" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D16">
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="77" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="78" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D19">
-    <cfRule type="cellIs" dxfId="75" priority="75" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="75" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="76" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D21">
-    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="73" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="71" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="72" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E18">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="69" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="70" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E22">
-    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="67" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="68" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F21">
-    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="65" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="66" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="64" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="61" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="62" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="59" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:G22">
-    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:G24">
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="56" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8:Z11 O4:S7 U4:Z7">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:T7">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB8:AM11 AB4:AF7 AH4:AM7">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG7">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB19:AG28">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB29:AG30">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>